<commit_message>
dal som graf do doku
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smuco/Desktop/xIAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79C4E82B-A094-A448-9350-1C6671C08C35}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C710099E-A627-434C-8A63-7D40DC843CA4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{EA81CAC7-B971-C547-A1D8-B2987245D83D}"/>
+    <workbookView xWindow="38400" yWindow="-10760" windowWidth="33600" windowHeight="21000" xr2:uid="{EA81CAC7-B971-C547-A1D8-B2987245D83D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,27 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Hárok1!$H$9:$H$13</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Hárok1!$L$9:$L$14</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Hárok1!$L$9:$L$14</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Hárok1!$L$9:$L$14</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Hárok1!$L$9:$L$14</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Hárok1!$L$8</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Hárok1!$L$9:$L$14</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Hárok1!$H$9:$H$13</definedName>
@@ -27,7 +47,7 @@
     <definedName name="_xlchart.v1.8" hidden="1">Hárok1!$L$8</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Hárok1!$L$9:$L$14</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,22 +62,25 @@
     <t>Matica</t>
   </si>
   <si>
-    <t>Teoretická zložitosť</t>
-  </si>
-  <si>
-    <t>Priemer výpočtového času [ s ]</t>
-  </si>
-  <si>
     <t>Počet hrán - E</t>
   </si>
   <si>
     <t>Počet uzlov - N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teoretická zložitosť [ - ] </t>
+  </si>
+  <si>
+    <t>Priemer výpočtového času [ ms ]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -223,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -234,6 +257,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -328,90 +353,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hárok1!$K$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Teoretická zložitosť</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hárok1!$H$9:$H$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hárok1!$K$9:$K$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2983.1372560199598</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>838787.96981771966</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C3D9-5545-8B76-9335C832C51E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="1"/>
@@ -421,7 +365,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Priemer výpočtového času [ s ]</c:v>
+                  <c:v>Priemer výpočtového času [ ms ]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -436,9 +380,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Hárok1!$H$9:$H$13</c:f>
               <c:numCache>
@@ -461,20 +417,32 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Hárok1!$L$9:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.2000000000000003E-2</c:v>
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5409999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4960000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1159999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C3D9-5545-8B76-9335C832C51E}"/>
@@ -489,14 +457,122 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="15675712"/>
         <c:axId val="15511264"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hárok1!$K$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Teoretická zložitosť [ - ] </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hárok1!$H$9:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hárok1!$K$9:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2983.1372560199598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22528.738020549157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67484.118501719699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128596.77265955749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>199779.41115163945</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C3D9-5545-8B76-9335C832C51E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="184459904"/>
+        <c:axId val="184458208"/>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="15675712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -539,11 +615,9 @@
         </c:txPr>
         <c:crossAx val="15511264"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="15511264"/>
         <c:scaling>
@@ -565,6 +639,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Priemer výpočtového času [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sk-SK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -598,7 +727,126 @@
         </c:txPr>
         <c:crossAx val="15675712"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="184458208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Teoretická</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="sk-SK" baseline="0"/>
+                  <a:t> zložitosť [-]</a:t>
+                </a:r>
+                <a:endParaRPr lang="sk-SK"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sk-SK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="184459904"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="50000"/>
+        <c:minorUnit val="10000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="184459904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184458208"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1243,16 +1491,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1225550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1579,16 +1827,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C8AA7D-F47F-3942-8D2E-006A09A5AE10}">
   <dimension ref="H7:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
-    <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="8:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1597,19 +1846,19 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="9" spans="8:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H9" s="4">
         <v>1</v>
       </c>
@@ -1619,65 +1868,85 @@
       <c r="J9" s="5">
         <v>70</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="10">
         <f t="shared" ref="K9:K12" si="0">I9*J9*LOG(J9) + I9^2</f>
         <v>2983.1372560199598</v>
       </c>
       <c r="L9" s="6">
-        <v>4.2000000000000003E-2</v>
+        <v>0.159</v>
       </c>
     </row>
-    <row r="10" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H10" s="4">
         <v>2</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="8" t="e">
+      <c r="I10" s="5">
+        <v>50</v>
+      </c>
+      <c r="J10" s="5">
+        <v>178</v>
+      </c>
+      <c r="K10" s="10">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L10" s="6"/>
+        <v>22528.738020549157</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.89800000000000002</v>
+      </c>
     </row>
-    <row r="11" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H11" s="4">
         <v>3</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="8" t="e">
+      <c r="I11" s="5">
+        <v>80</v>
+      </c>
+      <c r="J11" s="5">
+        <v>307</v>
+      </c>
+      <c r="K11" s="10">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L11" s="6"/>
+        <v>67484.118501719699</v>
+      </c>
+      <c r="L11" s="6">
+        <v>2.5409999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H12" s="4">
         <v>4</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="8" t="e">
+      <c r="I12" s="5">
+        <v>110</v>
+      </c>
+      <c r="J12" s="5">
+        <v>406</v>
+      </c>
+      <c r="K12" s="10">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L12" s="6"/>
+        <v>128596.77265955749</v>
+      </c>
+      <c r="L12" s="6">
+        <v>4.4960000000000004</v>
+      </c>
     </row>
-    <row r="13" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H13" s="7">
         <v>5</v>
       </c>
       <c r="I13" s="8">
-        <v>255</v>
+        <v>140</v>
       </c>
       <c r="J13" s="8">
-        <v>1010</v>
-      </c>
-      <c r="K13" s="8">
+        <v>480</v>
+      </c>
+      <c r="K13" s="11">
         <f>I13*J13*LOG(J13) + I13^2</f>
-        <v>838787.96981771966</v>
-      </c>
-      <c r="L13" s="9"/>
+        <v>199779.41115163945</v>
+      </c>
+      <c r="L13" s="9">
+        <v>6.1159999999999997</v>
+      </c>
     </row>
     <row r="14" spans="8:12" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>

<commit_message>
Úpravy z master vetvy
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smuco/Desktop/xIAL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{79C4E82B-A094-A448-9350-1C6671C08C35}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C710099E-A627-434C-8A63-7D40DC843CA4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{EA81CAC7-B971-C547-A1D8-B2987245D83D}"/>
+    <workbookView xWindow="38400" yWindow="-10760" windowWidth="33600" windowHeight="21000" xr2:uid="{EA81CAC7-B971-C547-A1D8-B2987245D83D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,27 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Hárok1!$H$9:$H$13</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Hárok1!$L$9:$L$14</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Hárok1!$L$9:$L$14</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Hárok1!$L$9:$L$14</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Hárok1!$H$9:$H$13</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Hárok1!$K$8</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Hárok1!$K$9:$K$13</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Hárok1!$L$8</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Hárok1!$L$9:$L$14</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Hárok1!$L$8</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Hárok1!$L$9:$L$14</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Hárok1!$H$9:$H$13</definedName>
@@ -27,7 +47,7 @@
     <definedName name="_xlchart.v1.8" hidden="1">Hárok1!$L$8</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Hárok1!$L$9:$L$14</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,22 +62,25 @@
     <t>Matica</t>
   </si>
   <si>
-    <t>Teoretická zložitosť</t>
-  </si>
-  <si>
-    <t>Priemer výpočtového času [ s ]</t>
-  </si>
-  <si>
     <t>Počet hrán - E</t>
   </si>
   <si>
     <t>Počet uzlov - N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teoretická zložitosť [ - ] </t>
+  </si>
+  <si>
+    <t>Priemer výpočtového času [ ms ]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -223,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -234,6 +257,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -328,90 +353,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Hárok1!$K$8</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Teoretická zložitosť</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Hárok1!$H$9:$H$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Hárok1!$K$9:$K$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2983.1372560199598</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>838787.96981771966</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-C3D9-5545-8B76-9335C832C51E}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="1"/>
@@ -421,7 +365,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Priemer výpočtového času [ s ]</c:v>
+                  <c:v>Priemer výpočtového času [ ms ]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -436,9 +380,21 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
               <c:f>Hárok1!$H$9:$H$13</c:f>
               <c:numCache>
@@ -461,20 +417,32 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
               <c:f>Hárok1!$L$9:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.2000000000000003E-2</c:v>
+                  <c:v>0.159</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.89800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5409999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4960000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1159999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C3D9-5545-8B76-9335C832C51E}"/>
@@ -489,14 +457,122 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
         <c:axId val="15675712"/>
         <c:axId val="15511264"/>
-      </c:lineChart>
-      <c:catAx>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hárok1!$K$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Teoretická zložitosť [ - ] </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hárok1!$H$9:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hárok1!$K$9:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2983.1372560199598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22528.738020549157</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67484.118501719699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>128596.77265955749</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>199779.41115163945</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C3D9-5545-8B76-9335C832C51E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="184459904"/>
+        <c:axId val="184458208"/>
+      </c:scatterChart>
+      <c:valAx>
         <c:axId val="15675712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -539,11 +615,9 @@
         </c:txPr>
         <c:crossAx val="15511264"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
       <c:valAx>
         <c:axId val="15511264"/>
         <c:scaling>
@@ -565,6 +639,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Priemer výpočtového času [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sk-SK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -598,7 +727,126 @@
         </c:txPr>
         <c:crossAx val="15675712"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="184458208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="sk-SK"/>
+                  <a:t>Teoretická</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="sk-SK" baseline="0"/>
+                  <a:t> zložitosť [-]</a:t>
+                </a:r>
+                <a:endParaRPr lang="sk-SK"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="sk-SK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="sk-SK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="184459904"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="50000"/>
+        <c:minorUnit val="10000"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="184459904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="184458208"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1243,16 +1491,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1225550</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1579,16 +1827,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C8AA7D-F47F-3942-8D2E-006A09A5AE10}">
   <dimension ref="H7:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17.1640625" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" customWidth="1"/>
-    <col min="12" max="12" width="26.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
+    <col min="12" max="12" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="8:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -1597,19 +1846,19 @@
         <v>0</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="9" spans="8:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H9" s="4">
         <v>1</v>
       </c>
@@ -1619,65 +1868,85 @@
       <c r="J9" s="5">
         <v>70</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="10">
         <f t="shared" ref="K9:K12" si="0">I9*J9*LOG(J9) + I9^2</f>
         <v>2983.1372560199598</v>
       </c>
       <c r="L9" s="6">
-        <v>4.2000000000000003E-2</v>
+        <v>0.159</v>
       </c>
     </row>
-    <row r="10" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H10" s="4">
         <v>2</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="8" t="e">
+      <c r="I10" s="5">
+        <v>50</v>
+      </c>
+      <c r="J10" s="5">
+        <v>178</v>
+      </c>
+      <c r="K10" s="10">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L10" s="6"/>
+        <v>22528.738020549157</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.89800000000000002</v>
+      </c>
     </row>
-    <row r="11" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H11" s="4">
         <v>3</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="8" t="e">
+      <c r="I11" s="5">
+        <v>80</v>
+      </c>
+      <c r="J11" s="5">
+        <v>307</v>
+      </c>
+      <c r="K11" s="10">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L11" s="6"/>
+        <v>67484.118501719699</v>
+      </c>
+      <c r="L11" s="6">
+        <v>2.5409999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="8:12" x14ac:dyDescent="0.2">
       <c r="H12" s="4">
         <v>4</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="8" t="e">
+      <c r="I12" s="5">
+        <v>110</v>
+      </c>
+      <c r="J12" s="5">
+        <v>406</v>
+      </c>
+      <c r="K12" s="10">
         <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="L12" s="6"/>
+        <v>128596.77265955749</v>
+      </c>
+      <c r="L12" s="6">
+        <v>4.4960000000000004</v>
+      </c>
     </row>
-    <row r="13" spans="8:12" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="8:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H13" s="7">
         <v>5</v>
       </c>
       <c r="I13" s="8">
-        <v>255</v>
+        <v>140</v>
       </c>
       <c r="J13" s="8">
-        <v>1010</v>
-      </c>
-      <c r="K13" s="8">
+        <v>480</v>
+      </c>
+      <c r="K13" s="11">
         <f>I13*J13*LOG(J13) + I13^2</f>
-        <v>838787.96981771966</v>
-      </c>
-      <c r="L13" s="9"/>
+        <v>199779.41115163945</v>
+      </c>
+      <c r="L13" s="9">
+        <v>6.1159999999999997</v>
+      </c>
     </row>
     <row r="14" spans="8:12" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>

</xml_diff>